<commit_message>
Update some responses and minor comments
</commit_message>
<xml_diff>
--- a/Todo_List.xlsx
+++ b/Todo_List.xlsx
@@ -4,11 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -224,12 +228,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -244,13 +254,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -268,6 +286,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,19 +753,19 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>1</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>100</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -758,21 +789,21 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>1</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D13" s="6">
+        <v>100</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -794,21 +825,21 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>1</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D15" s="6">
+        <v>100</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -902,55 +933,55 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>5</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>100</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="6">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>5</v>
       </c>
-      <c r="D22">
-        <v>50</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>250</v>
+      <c r="D22" s="6">
+        <v>100</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="0"/>
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>5</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>100</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
@@ -1160,15 +1191,30 @@
       </c>
       <c r="E35">
         <f>SUM(E2:E34)</f>
-        <v>3920</v>
+        <v>4370</v>
       </c>
       <c r="F35">
         <f>E35/C35</f>
-        <v>41.702127659574465</v>
+        <v>46.48936170212766</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Timepoints and some major trimming
</commit_message>
<xml_diff>
--- a/Todo_List.xlsx
+++ b/Todo_List.xlsx
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,21 +1115,21 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>5</v>
       </c>
-      <c r="D31">
-        <v>30</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>150</v>
+      <c r="D31" s="6">
+        <v>100</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="0"/>
+        <v>500</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,11 +1199,11 @@
       </c>
       <c r="E35">
         <f>SUM(E2:E34)</f>
-        <v>7240</v>
+        <v>7590</v>
       </c>
       <c r="F35">
         <f>E35/C35</f>
-        <v>76.21052631578948</v>
+        <v>79.89473684210526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update literature review (to finish)
</commit_message>
<xml_diff>
--- a/Todo_List.xlsx
+++ b/Todo_List.xlsx
@@ -563,7 +563,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,21 +605,21 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>1.2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="6">
+        <v>100</v>
+      </c>
+      <c r="E3" s="6">
         <f t="shared" ref="E3:E34" si="0">D3*C3</f>
-        <v>150</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -659,21 +659,21 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="4">
         <v>1.5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D6" s="6">
+        <v>100</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1199,11 +1199,11 @@
       </c>
       <c r="E35">
         <f>SUM(E2:E34)</f>
-        <v>7590</v>
+        <v>8140</v>
       </c>
       <c r="F35">
         <f>E35/C35</f>
-        <v>79.89473684210526</v>
+        <v>85.684210526315795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update some draft and update all pictures
</commit_message>
<xml_diff>
--- a/Todo_List.xlsx
+++ b/Todo_List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>Number</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>remake graph</t>
+  </si>
+  <si>
+    <t>Need reinstate</t>
   </si>
 </sst>
 </file>
@@ -560,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +865,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
@@ -880,7 +883,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
@@ -898,7 +901,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
@@ -916,7 +919,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
@@ -934,7 +937,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -952,7 +955,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -969,8 +972,11 @@
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -987,8 +993,11 @@
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>39</v>
       </c>
@@ -1005,8 +1014,11 @@
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>41</v>
       </c>
@@ -1024,7 +1036,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>43</v>
       </c>
@@ -1042,7 +1054,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>45</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>47</v>
       </c>
@@ -1078,7 +1090,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>49</v>
       </c>
@@ -1095,8 +1107,11 @@
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>50</v>
       </c>
@@ -1114,7 +1129,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>52</v>
       </c>
@@ -1132,7 +1147,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>